<commit_message>
Add vehicle related classes
</commit_message>
<xml_diff>
--- a/Document/Transport Data Dictionary.xlsx
+++ b/Document/Transport Data Dictionary.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project\QTrans\Document\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59312709-613E-44BC-840A-E08F2C44B0AE}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3ACA6A41-AB33-4536-ADBB-5FE819EC5B58}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20385" windowHeight="8370" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DataDic" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="vehicle" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="144525"/>
@@ -717,9 +717,6 @@
     <t>none/Install/Repair/falty</t>
   </si>
   <si>
-    <t>TblMstLocation</t>
-  </si>
-  <si>
     <t>FK, Ref to TblMstProduct</t>
   </si>
   <si>
@@ -754,6 +751,9 @@
   </si>
   <si>
     <t>msgid</t>
+  </si>
+  <si>
+    <t>TblLocation</t>
   </si>
 </sst>
 </file>
@@ -4260,6 +4260,16 @@
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="D2:F2"/>
+    <mergeCell ref="D31:F31"/>
+    <mergeCell ref="D47:F47"/>
+    <mergeCell ref="D54:F54"/>
+    <mergeCell ref="D61:F61"/>
+    <mergeCell ref="D70:F70"/>
+    <mergeCell ref="D87:F87"/>
+    <mergeCell ref="D101:F101"/>
+    <mergeCell ref="D116:F116"/>
+    <mergeCell ref="D122:F122"/>
     <mergeCell ref="D199:F199"/>
     <mergeCell ref="D210:F210"/>
     <mergeCell ref="D217:F217"/>
@@ -4269,16 +4279,6 @@
     <mergeCell ref="D168:F168"/>
     <mergeCell ref="D182:F182"/>
     <mergeCell ref="D190:F190"/>
-    <mergeCell ref="D70:F70"/>
-    <mergeCell ref="D87:F87"/>
-    <mergeCell ref="D101:F101"/>
-    <mergeCell ref="D116:F116"/>
-    <mergeCell ref="D122:F122"/>
-    <mergeCell ref="D2:F2"/>
-    <mergeCell ref="D31:F31"/>
-    <mergeCell ref="D47:F47"/>
-    <mergeCell ref="D54:F54"/>
-    <mergeCell ref="D61:F61"/>
   </mergeCells>
   <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>
@@ -4289,8 +4289,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B2:G73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="F73" sqref="F73"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D60" sqref="D60:F60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.5703125" defaultRowHeight="15"/>
@@ -4354,11 +4354,9 @@
         <v>85</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E5" s="3">
-        <v>20</v>
-      </c>
+        <v>92</v>
+      </c>
+      <c r="E5" s="3"/>
       <c r="F5" s="3" t="s">
         <v>10</v>
       </c>
@@ -4766,7 +4764,7 @@
         <v>212</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>213</v>
+        <v>77</v>
       </c>
       <c r="E37" s="3">
         <v>20</v>
@@ -4939,7 +4937,7 @@
       <c r="E50" s="3"/>
       <c r="F50" s="3"/>
       <c r="G50" s="3" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="51" spans="2:7">
@@ -5030,7 +5028,7 @@
         <v>0</v>
       </c>
       <c r="D60" s="16" t="s">
-        <v>231</v>
+        <v>243</v>
       </c>
       <c r="E60" s="16"/>
       <c r="F60" s="16"/>
@@ -5059,7 +5057,7 @@
     <row r="62" spans="2:7">
       <c r="B62" s="3"/>
       <c r="C62" s="3" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="D62" s="3" t="s">
         <v>108</v>
@@ -5081,16 +5079,16 @@
       <c r="E63" s="3"/>
       <c r="F63" s="3"/>
       <c r="G63" s="3" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="64" spans="2:7">
       <c r="B64" s="3"/>
       <c r="C64" s="4" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="D64" s="4" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="E64" s="3">
         <v>1</v>
@@ -5101,7 +5099,7 @@
     <row r="65" spans="2:7">
       <c r="B65" s="3"/>
       <c r="C65" s="4" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="D65" s="4" t="s">
         <v>77</v>
@@ -5115,7 +5113,7 @@
     <row r="66" spans="2:7">
       <c r="B66" s="3"/>
       <c r="C66" s="4" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="D66" s="3" t="s">
         <v>35</v>
@@ -5127,7 +5125,7 @@
     <row r="67" spans="2:7">
       <c r="B67" s="3"/>
       <c r="C67" s="4" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="D67" s="3" t="s">
         <v>35</v>
@@ -5139,7 +5137,7 @@
     <row r="68" spans="2:7">
       <c r="B68" s="3"/>
       <c r="C68" s="4" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="D68" s="3" t="s">
         <v>35</v>
@@ -5151,7 +5149,7 @@
     <row r="69" spans="2:7">
       <c r="B69" s="3"/>
       <c r="C69" s="4" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="D69" s="3" t="s">
         <v>35</v>
@@ -5163,7 +5161,7 @@
     <row r="70" spans="2:7">
       <c r="B70" s="3"/>
       <c r="C70" s="4" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="D70" s="3" t="s">
         <v>108</v>
@@ -5175,7 +5173,7 @@
     <row r="71" spans="2:7">
       <c r="B71" s="3"/>
       <c r="C71" s="4" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="D71" s="3" t="s">
         <v>28</v>
@@ -5187,7 +5185,7 @@
     <row r="72" spans="2:7">
       <c r="B72" s="3"/>
       <c r="C72" s="4" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="D72" s="3" t="s">
         <v>108</v>

</xml_diff>

<commit_message>
Add Trcuk cancellation API
</commit_message>
<xml_diff>
--- a/Document/Transport Data Dictionary.xlsx
+++ b/Document/Transport Data Dictionary.xlsx
@@ -11,12 +11,12 @@
     <sheet name="vehicle" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="144525" refMode="R1C1" concurrentCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279">
   <si>
     <t>Table Name</t>
   </si>
@@ -751,6 +751,87 @@
   </si>
   <si>
     <t>msgid</t>
+  </si>
+  <si>
+    <t>Table</t>
+  </si>
+  <si>
+    <t>TblMstAlert</t>
+  </si>
+  <si>
+    <t>ColumnName</t>
+  </si>
+  <si>
+    <t>AlertId</t>
+  </si>
+  <si>
+    <t>AlertType</t>
+  </si>
+  <si>
+    <t>(SMS, Email, Apps)</t>
+  </si>
+  <si>
+    <t>MsgType</t>
+  </si>
+  <si>
+    <t>1=Opt,2=PostAlert,3=TruckAssign.. etc</t>
+  </si>
+  <si>
+    <t>HTML</t>
+  </si>
+  <si>
+    <t>if Email than HTML enable</t>
+  </si>
+  <si>
+    <t>Small Int</t>
+  </si>
+  <si>
+    <t>0=None,1=Send,2=fail,3=Inprogress</t>
+  </si>
+  <si>
+    <t>UpdateDate</t>
+  </si>
+  <si>
+    <t>TblMstTruckAssignment</t>
+  </si>
+  <si>
+    <t>TruckRequestId</t>
+  </si>
+  <si>
+    <t>BigInt</t>
+  </si>
+  <si>
+    <t>PK Auto generator</t>
+  </si>
+  <si>
+    <t>refe ID</t>
+  </si>
+  <si>
+    <t>RegistrationNo</t>
+  </si>
+  <si>
+    <t>Varchar(30)</t>
+  </si>
+  <si>
+    <t>Number plat</t>
+  </si>
+  <si>
+    <t>DriverName</t>
+  </si>
+  <si>
+    <t>Varchar(50)</t>
+  </si>
+  <si>
+    <t>Varchar(12)</t>
+  </si>
+  <si>
+    <t>small int</t>
+  </si>
+  <si>
+    <t>0=None,1=pending,2=Approve,3=Reject,4=Cancel</t>
+  </si>
+  <si>
+    <t>Varchar(200)</t>
   </si>
   <si>
     <t>connector.AddInParameterWithValue("@</t>
@@ -815,14 +896,38 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -837,93 +942,8 @@
     </font>
     <font>
       <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -943,8 +963,16 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -957,13 +985,78 @@
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="34">
+  <fills count="36">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -973,7 +1066,85 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -991,19 +1162,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
+        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1015,25 +1174,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
+        <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1051,25 +1210,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1081,37 +1228,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1123,37 +1240,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1182,6 +1275,15 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -1197,11 +1299,56 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4"/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1225,64 +1372,10 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1300,134 +1393,134 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="18" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="14" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="12" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="26" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="17" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="17" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1437,7 +1530,11 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1445,11 +1542,11 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1852,7 +1949,7 @@
       </c>
     </row>
     <row r="4" spans="2:7">
-      <c r="B4" s="8">
+      <c r="B4" s="12">
         <v>1</v>
       </c>
       <c r="C4" s="1" t="s">
@@ -1870,7 +1967,7 @@
       </c>
     </row>
     <row r="5" spans="2:7">
-      <c r="B5" s="8">
+      <c r="B5" s="12">
         <v>2</v>
       </c>
       <c r="C5" s="1" t="s">
@@ -1890,7 +1987,7 @@
       </c>
     </row>
     <row r="6" spans="2:7">
-      <c r="B6" s="8">
+      <c r="B6" s="12">
         <v>3</v>
       </c>
       <c r="C6" s="1" t="s">
@@ -1910,7 +2007,7 @@
       </c>
     </row>
     <row r="7" spans="2:7">
-      <c r="B7" s="8">
+      <c r="B7" s="12">
         <v>4</v>
       </c>
       <c r="C7" s="1" t="s">
@@ -1930,7 +2027,7 @@
       </c>
     </row>
     <row r="8" spans="2:7">
-      <c r="B8" s="8">
+      <c r="B8" s="12">
         <v>5</v>
       </c>
       <c r="C8" s="1" t="s">
@@ -1950,7 +2047,7 @@
       </c>
     </row>
     <row r="9" spans="2:7">
-      <c r="B9" s="8"/>
+      <c r="B9" s="12"/>
       <c r="C9" s="1" t="s">
         <v>22</v>
       </c>
@@ -1966,7 +2063,7 @@
       <c r="G9" s="1"/>
     </row>
     <row r="10" spans="2:7">
-      <c r="B10" s="8">
+      <c r="B10" s="12">
         <v>6</v>
       </c>
       <c r="C10" s="1" t="s">
@@ -1986,7 +2083,7 @@
       </c>
     </row>
     <row r="11" spans="2:7">
-      <c r="B11" s="8">
+      <c r="B11" s="12">
         <v>7</v>
       </c>
       <c r="C11" s="1" t="s">
@@ -2006,7 +2103,7 @@
       </c>
     </row>
     <row r="12" spans="2:7">
-      <c r="B12" s="8">
+      <c r="B12" s="12">
         <v>8</v>
       </c>
       <c r="C12" s="1" t="s">
@@ -2024,7 +2121,7 @@
       </c>
     </row>
     <row r="13" spans="2:7">
-      <c r="B13" s="8">
+      <c r="B13" s="12">
         <v>9</v>
       </c>
       <c r="C13" s="1" t="s">
@@ -2044,7 +2141,7 @@
       </c>
     </row>
     <row r="14" spans="2:7">
-      <c r="B14" s="8">
+      <c r="B14" s="12">
         <v>10</v>
       </c>
       <c r="C14" s="1" t="s">
@@ -2064,7 +2161,7 @@
       </c>
     </row>
     <row r="15" spans="2:7">
-      <c r="B15" s="8">
+      <c r="B15" s="12">
         <v>11</v>
       </c>
       <c r="C15" s="1" t="s">
@@ -2082,7 +2179,7 @@
       </c>
     </row>
     <row r="16" spans="2:7">
-      <c r="B16" s="8">
+      <c r="B16" s="12">
         <v>12</v>
       </c>
       <c r="C16" s="1" t="s">
@@ -2102,7 +2199,7 @@
       </c>
     </row>
     <row r="17" spans="2:7">
-      <c r="B17" s="8">
+      <c r="B17" s="12">
         <v>13</v>
       </c>
       <c r="C17" s="1" t="s">
@@ -2122,7 +2219,7 @@
       </c>
     </row>
     <row r="18" spans="2:7">
-      <c r="B18" s="8">
+      <c r="B18" s="12">
         <v>14</v>
       </c>
       <c r="C18" s="1" t="s">
@@ -2142,7 +2239,7 @@
       </c>
     </row>
     <row r="19" spans="2:7">
-      <c r="B19" s="8">
+      <c r="B19" s="12">
         <v>15</v>
       </c>
       <c r="C19" s="1" t="s">
@@ -2162,7 +2259,7 @@
       </c>
     </row>
     <row r="20" spans="2:7">
-      <c r="B20" s="8">
+      <c r="B20" s="12">
         <v>16</v>
       </c>
       <c r="C20" s="1" t="s">
@@ -2182,7 +2279,7 @@
       </c>
     </row>
     <row r="21" spans="2:7">
-      <c r="B21" s="8">
+      <c r="B21" s="12">
         <v>17</v>
       </c>
       <c r="C21" s="1" t="s">
@@ -2202,7 +2299,7 @@
       </c>
     </row>
     <row r="22" spans="2:7">
-      <c r="B22" s="8"/>
+      <c r="B22" s="12"/>
       <c r="C22" s="1" t="s">
         <v>45</v>
       </c>
@@ -2218,7 +2315,7 @@
       </c>
     </row>
     <row r="23" spans="2:7">
-      <c r="B23" s="8"/>
+      <c r="B23" s="12"/>
       <c r="C23" s="1" t="s">
         <v>48</v>
       </c>
@@ -2234,7 +2331,7 @@
       </c>
     </row>
     <row r="24" spans="2:7">
-      <c r="B24" s="8">
+      <c r="B24" s="12">
         <v>18</v>
       </c>
       <c r="C24" s="1" t="s">
@@ -2254,7 +2351,7 @@
       </c>
     </row>
     <row r="25" spans="2:7">
-      <c r="B25" s="8">
+      <c r="B25" s="12">
         <v>19</v>
       </c>
       <c r="C25" s="1" t="s">
@@ -2274,7 +2371,7 @@
       </c>
     </row>
     <row r="26" spans="2:7">
-      <c r="B26" s="8">
+      <c r="B26" s="12">
         <v>20</v>
       </c>
       <c r="C26" s="1" t="s">
@@ -2292,7 +2389,7 @@
       </c>
     </row>
     <row r="27" spans="2:7">
-      <c r="B27" s="8">
+      <c r="B27" s="12">
         <v>21</v>
       </c>
       <c r="C27" s="4" t="s">
@@ -2308,7 +2405,7 @@
       <c r="G27" s="1"/>
     </row>
     <row r="28" spans="2:7">
-      <c r="B28" s="8">
+      <c r="B28" s="12">
         <v>22</v>
       </c>
       <c r="C28" s="4" t="s">
@@ -2605,7 +2702,7 @@
       <c r="F50" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="G50" s="9" t="s">
+      <c r="G50" s="13" t="s">
         <v>69</v>
       </c>
     </row>
@@ -2642,96 +2739,96 @@
       </c>
     </row>
     <row r="53" spans="2:7">
-      <c r="B53" s="10"/>
-      <c r="C53" s="10"/>
-      <c r="D53" s="10"/>
-      <c r="E53" s="10"/>
-      <c r="F53" s="10"/>
-      <c r="G53" s="10"/>
+      <c r="B53" s="14"/>
+      <c r="C53" s="14"/>
+      <c r="D53" s="14"/>
+      <c r="E53" s="14"/>
+      <c r="F53" s="14"/>
+      <c r="G53" s="14"/>
     </row>
     <row r="54" spans="2:7">
-      <c r="B54" s="11"/>
-      <c r="C54" s="11" t="s">
+      <c r="B54" s="15"/>
+      <c r="C54" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="D54" s="12" t="s">
+      <c r="D54" s="16" t="s">
         <v>73</v>
       </c>
-      <c r="E54" s="12"/>
-      <c r="F54" s="12"/>
-      <c r="G54" s="11" t="s">
+      <c r="E54" s="16"/>
+      <c r="F54" s="16"/>
+      <c r="G54" s="15" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="55" spans="2:7">
-      <c r="B55" s="11" t="s">
+      <c r="B55" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="C55" s="11" t="s">
+      <c r="C55" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="D55" s="11" t="s">
+      <c r="D55" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="E55" s="11" t="s">
+      <c r="E55" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="F55" s="11" t="s">
+      <c r="F55" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="G55" s="11" t="s">
+      <c r="G55" s="15" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="56" spans="2:7">
-      <c r="B56" s="13"/>
-      <c r="C56" s="13" t="s">
+      <c r="B56" s="17"/>
+      <c r="C56" s="17" t="s">
         <v>75</v>
       </c>
-      <c r="D56" s="13"/>
-      <c r="E56" s="13"/>
-      <c r="F56" s="13"/>
-      <c r="G56" s="13" t="s">
+      <c r="D56" s="17"/>
+      <c r="E56" s="17"/>
+      <c r="F56" s="17"/>
+      <c r="G56" s="17" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="57" spans="2:7">
-      <c r="B57" s="13"/>
-      <c r="C57" s="13" t="s">
+      <c r="B57" s="17"/>
+      <c r="C57" s="17" t="s">
         <v>76</v>
       </c>
-      <c r="D57" s="13" t="s">
+      <c r="D57" s="17" t="s">
         <v>77</v>
       </c>
-      <c r="E57" s="13">
+      <c r="E57" s="17">
         <v>20</v>
       </c>
-      <c r="F57" s="13"/>
-      <c r="G57" s="13" t="s">
+      <c r="F57" s="17"/>
+      <c r="G57" s="17" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="58" spans="2:7">
-      <c r="B58" s="13"/>
-      <c r="C58" s="13" t="s">
+      <c r="B58" s="17"/>
+      <c r="C58" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="D58" s="13" t="s">
+      <c r="D58" s="17" t="s">
         <v>77</v>
       </c>
-      <c r="E58" s="13">
+      <c r="E58" s="17">
         <v>200</v>
       </c>
-      <c r="F58" s="13"/>
-      <c r="G58" s="13"/>
+      <c r="F58" s="17"/>
+      <c r="G58" s="17"/>
     </row>
     <row r="59" spans="2:7">
-      <c r="B59" s="10"/>
+      <c r="B59" s="14"/>
       <c r="C59" s="3"/>
-      <c r="D59" s="10"/>
-      <c r="E59" s="10"/>
-      <c r="F59" s="10"/>
-      <c r="G59" s="10"/>
+      <c r="D59" s="14"/>
+      <c r="E59" s="14"/>
+      <c r="F59" s="14"/>
+      <c r="G59" s="14"/>
     </row>
     <row r="61" spans="2:7">
       <c r="B61" s="5"/>
@@ -2767,7 +2864,7 @@
     </row>
     <row r="63" spans="2:7">
       <c r="B63" s="5"/>
-      <c r="C63" s="14" t="s">
+      <c r="C63" s="18" t="s">
         <v>80</v>
       </c>
       <c r="D63" s="1" t="s">
@@ -2783,7 +2880,7 @@
     </row>
     <row r="64" spans="2:7">
       <c r="B64" s="5"/>
-      <c r="C64" s="14" t="s">
+      <c r="C64" s="18" t="s">
         <v>8</v>
       </c>
       <c r="D64" s="1" t="s">
@@ -2799,7 +2896,7 @@
     </row>
     <row r="65" spans="2:7">
       <c r="B65" s="5"/>
-      <c r="C65" s="14" t="s">
+      <c r="C65" s="18" t="s">
         <v>56</v>
       </c>
       <c r="D65" s="1" t="s">
@@ -3267,7 +3364,7 @@
       </c>
       <c r="E101" s="6"/>
       <c r="F101" s="6"/>
-      <c r="G101" s="14" t="s">
+      <c r="G101" s="18" t="s">
         <v>106</v>
       </c>
     </row>
@@ -3317,7 +3414,7 @@
         <v>10</v>
       </c>
       <c r="F104" s="1"/>
-      <c r="G104" s="15" t="s">
+      <c r="G104" s="19" t="s">
         <v>110</v>
       </c>
     </row>
@@ -3443,20 +3540,20 @@
       <c r="G113" s="1"/>
     </row>
     <row r="114" spans="2:7">
-      <c r="B114" s="10"/>
+      <c r="B114" s="14"/>
       <c r="C114" s="3"/>
       <c r="D114" s="3"/>
-      <c r="E114" s="10"/>
-      <c r="F114" s="10"/>
-      <c r="G114" s="10"/>
+      <c r="E114" s="14"/>
+      <c r="F114" s="14"/>
+      <c r="G114" s="14"/>
     </row>
     <row r="115" spans="2:7">
-      <c r="B115" s="10"/>
+      <c r="B115" s="14"/>
       <c r="C115" s="3"/>
       <c r="D115" s="3"/>
-      <c r="E115" s="10"/>
-      <c r="F115" s="10"/>
-      <c r="G115" s="10"/>
+      <c r="E115" s="14"/>
+      <c r="F115" s="14"/>
+      <c r="G115" s="14"/>
     </row>
     <row r="116" spans="2:7">
       <c r="B116" s="5"/>
@@ -3491,44 +3588,44 @@
       </c>
     </row>
     <row r="118" spans="2:7">
-      <c r="B118" s="14"/>
-      <c r="C118" s="14" t="s">
+      <c r="B118" s="18"/>
+      <c r="C118" s="18" t="s">
         <v>116</v>
       </c>
-      <c r="D118" s="14" t="s">
+      <c r="D118" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="E118" s="14"/>
-      <c r="F118" s="14"/>
+      <c r="E118" s="18"/>
+      <c r="F118" s="18"/>
       <c r="G118" s="1" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="119" spans="2:7">
-      <c r="B119" s="14"/>
-      <c r="C119" s="14" t="s">
+      <c r="B119" s="18"/>
+      <c r="C119" s="18" t="s">
         <v>120</v>
       </c>
-      <c r="D119" s="14" t="s">
+      <c r="D119" s="18" t="s">
         <v>77</v>
       </c>
-      <c r="E119" s="14"/>
-      <c r="F119" s="14">
+      <c r="E119" s="18"/>
+      <c r="F119" s="18">
         <v>50</v>
       </c>
-      <c r="G119" s="14" t="s">
+      <c r="G119" s="18" t="s">
         <v>121</v>
       </c>
     </row>
     <row r="120" spans="2:7">
-      <c r="B120" s="14"/>
-      <c r="C120" s="16" t="s">
+      <c r="B120" s="18"/>
+      <c r="C120" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="D120" s="14"/>
-      <c r="E120" s="14"/>
-      <c r="F120" s="14"/>
-      <c r="G120" s="14"/>
+      <c r="D120" s="18"/>
+      <c r="E120" s="18"/>
+      <c r="F120" s="18"/>
+      <c r="G120" s="18"/>
     </row>
     <row r="122" spans="2:7">
       <c r="B122" s="5"/>
@@ -3563,60 +3660,60 @@
       </c>
     </row>
     <row r="124" spans="2:7">
-      <c r="B124" s="14"/>
-      <c r="C124" s="14" t="s">
+      <c r="B124" s="18"/>
+      <c r="C124" s="18" t="s">
         <v>113</v>
       </c>
-      <c r="D124" s="14" t="s">
+      <c r="D124" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="E124" s="14"/>
-      <c r="F124" s="14"/>
+      <c r="E124" s="18"/>
+      <c r="F124" s="18"/>
       <c r="G124" s="1" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="125" spans="2:7">
-      <c r="B125" s="14"/>
-      <c r="C125" s="14" t="s">
+      <c r="B125" s="18"/>
+      <c r="C125" s="18" t="s">
         <v>123</v>
       </c>
-      <c r="D125" s="14" t="s">
+      <c r="D125" s="18" t="s">
         <v>77</v>
       </c>
-      <c r="E125" s="14"/>
-      <c r="F125" s="14">
+      <c r="E125" s="18"/>
+      <c r="F125" s="18">
         <v>50</v>
       </c>
-      <c r="G125" s="14" t="s">
+      <c r="G125" s="18" t="s">
         <v>124</v>
       </c>
     </row>
     <row r="126" spans="2:7">
-      <c r="B126" s="14"/>
-      <c r="C126" s="16" t="s">
+      <c r="B126" s="18"/>
+      <c r="C126" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="D126" s="14"/>
-      <c r="E126" s="14"/>
-      <c r="F126" s="14"/>
-      <c r="G126" s="14"/>
+      <c r="D126" s="18"/>
+      <c r="E126" s="18"/>
+      <c r="F126" s="18"/>
+      <c r="G126" s="18"/>
     </row>
     <row r="127" spans="2:7">
-      <c r="B127" s="17"/>
-      <c r="C127" s="18"/>
-      <c r="D127" s="17"/>
-      <c r="E127" s="17"/>
-      <c r="F127" s="17"/>
-      <c r="G127" s="17"/>
+      <c r="B127" s="21"/>
+      <c r="C127" s="22"/>
+      <c r="D127" s="21"/>
+      <c r="E127" s="21"/>
+      <c r="F127" s="21"/>
+      <c r="G127" s="21"/>
     </row>
     <row r="128" spans="2:7">
-      <c r="B128" s="17"/>
-      <c r="C128" s="18"/>
-      <c r="D128" s="17"/>
-      <c r="E128" s="17"/>
-      <c r="F128" s="17"/>
-      <c r="G128" s="17"/>
+      <c r="B128" s="21"/>
+      <c r="C128" s="22"/>
+      <c r="D128" s="21"/>
+      <c r="E128" s="21"/>
+      <c r="F128" s="21"/>
+      <c r="G128" s="21"/>
     </row>
     <row r="129" spans="2:7">
       <c r="B129" s="5"/>
@@ -3651,44 +3748,44 @@
       </c>
     </row>
     <row r="131" spans="2:7">
-      <c r="B131" s="14"/>
-      <c r="C131" s="14" t="s">
+      <c r="B131" s="18"/>
+      <c r="C131" s="18" t="s">
         <v>126</v>
       </c>
-      <c r="D131" s="14" t="s">
+      <c r="D131" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="E131" s="14"/>
-      <c r="F131" s="14"/>
+      <c r="E131" s="18"/>
+      <c r="F131" s="18"/>
       <c r="G131" s="1" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="132" spans="2:7">
-      <c r="B132" s="14"/>
-      <c r="C132" s="14" t="s">
+      <c r="B132" s="18"/>
+      <c r="C132" s="18" t="s">
         <v>85</v>
       </c>
-      <c r="D132" s="14" t="s">
+      <c r="D132" s="18" t="s">
         <v>77</v>
       </c>
-      <c r="E132" s="14"/>
-      <c r="F132" s="14">
+      <c r="E132" s="18"/>
+      <c r="F132" s="18">
         <v>50</v>
       </c>
-      <c r="G132" s="14" t="s">
+      <c r="G132" s="18" t="s">
         <v>127</v>
       </c>
     </row>
     <row r="133" spans="2:7">
-      <c r="B133" s="14"/>
-      <c r="C133" s="16" t="s">
+      <c r="B133" s="18"/>
+      <c r="C133" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="D133" s="14"/>
-      <c r="E133" s="14"/>
-      <c r="F133" s="14"/>
-      <c r="G133" s="14"/>
+      <c r="D133" s="18"/>
+      <c r="E133" s="18"/>
+      <c r="F133" s="18"/>
+      <c r="G133" s="18"/>
     </row>
     <row r="135" spans="2:7">
       <c r="B135" s="5"/>
@@ -3700,7 +3797,7 @@
       </c>
       <c r="E135" s="6"/>
       <c r="F135" s="6"/>
-      <c r="G135" s="14" t="s">
+      <c r="G135" s="18" t="s">
         <v>106</v>
       </c>
     </row>
@@ -3879,16 +3976,16 @@
       <c r="G146" s="1"/>
     </row>
     <row r="147" spans="2:7">
-      <c r="B147" s="13"/>
-      <c r="C147" s="13" t="s">
+      <c r="B147" s="17"/>
+      <c r="C147" s="17" t="s">
         <v>144</v>
       </c>
-      <c r="D147" s="13" t="s">
+      <c r="D147" s="17" t="s">
         <v>145</v>
       </c>
-      <c r="E147" s="13"/>
-      <c r="F147" s="13"/>
-      <c r="G147" s="13" t="s">
+      <c r="E147" s="17"/>
+      <c r="F147" s="17"/>
+      <c r="G147" s="17" t="s">
         <v>146</v>
       </c>
     </row>
@@ -3904,7 +4001,7 @@
       <c r="F148" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="G148" s="9" t="s">
+      <c r="G148" s="13" t="s">
         <v>148</v>
       </c>
     </row>
@@ -3920,7 +4017,7 @@
       <c r="F149" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="G149" s="9" t="s">
+      <c r="G149" s="13" t="s">
         <v>150</v>
       </c>
     </row>
@@ -3936,7 +4033,7 @@
       <c r="F150" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="G150" s="9" t="s">
+      <c r="G150" s="13" t="s">
         <v>152</v>
       </c>
     </row>
@@ -4167,8 +4264,8 @@
     <row r="166" spans="3:7">
       <c r="C166" s="3"/>
       <c r="D166" s="3"/>
-      <c r="E166" s="10"/>
-      <c r="F166" s="10"/>
+      <c r="E166" s="14"/>
+      <c r="F166" s="14"/>
       <c r="G166" s="3"/>
     </row>
     <row r="168" spans="2:7">
@@ -4313,7 +4410,7 @@
       </c>
       <c r="E177" s="1"/>
       <c r="F177" s="1"/>
-      <c r="G177" s="9" t="s">
+      <c r="G177" s="13" t="s">
         <v>183</v>
       </c>
     </row>
@@ -4930,16 +5027,17 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="B2:G73"/>
+  <dimension ref="B2:G100"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B57" sqref="B57"/>
+    <sheetView tabSelected="1" topLeftCell="A74" workbookViewId="0">
+      <selection activeCell="G87" sqref="G87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.5714285714286" defaultRowHeight="15" outlineLevelCol="6"/>
   <cols>
     <col min="2" max="2" width="5.42857142857143" customWidth="1"/>
     <col min="3" max="3" width="24.1428571428571" customWidth="1"/>
+    <col min="4" max="4" width="24.4285714285714" customWidth="1"/>
     <col min="7" max="7" width="23.5714285714286" customWidth="1"/>
   </cols>
   <sheetData>
@@ -5681,7 +5779,7 @@
       <c r="G56" s="1"/>
     </row>
     <row r="57" spans="2:7">
-      <c r="B57" s="7"/>
+      <c r="B57" s="1"/>
       <c r="C57" s="1" t="s">
         <v>232</v>
       </c>
@@ -5877,6 +5975,349 @@
       <c r="E73" s="1"/>
       <c r="F73" s="1"/>
       <c r="G73" s="1"/>
+    </row>
+    <row r="76" spans="3:5">
+      <c r="C76" s="7" t="s">
+        <v>245</v>
+      </c>
+      <c r="D76" s="7" t="s">
+        <v>246</v>
+      </c>
+      <c r="E76" s="8"/>
+    </row>
+    <row r="77" spans="3:7">
+      <c r="C77" s="9" t="s">
+        <v>247</v>
+      </c>
+      <c r="D77" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="E77" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="F77" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="G77" s="9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="78" spans="3:7">
+      <c r="C78" s="8" t="s">
+        <v>248</v>
+      </c>
+      <c r="D78" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="E78" s="8"/>
+      <c r="F78" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="G78" s="8"/>
+    </row>
+    <row r="79" spans="3:7">
+      <c r="C79" s="8" t="s">
+        <v>249</v>
+      </c>
+      <c r="D79" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="E79" s="8"/>
+      <c r="F79" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="G79" s="8" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="80" spans="3:7">
+      <c r="C80" s="8" t="s">
+        <v>251</v>
+      </c>
+      <c r="D80" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="E80" s="8"/>
+      <c r="F80" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="G80" s="8" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="81" spans="3:7">
+      <c r="C81" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="D81" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="E81" s="8" t="s">
+        <v>115</v>
+      </c>
+      <c r="F81" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="G81" s="8"/>
+    </row>
+    <row r="82" spans="3:7">
+      <c r="C82" s="8" t="s">
+        <v>253</v>
+      </c>
+      <c r="D82" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="E82" s="8"/>
+      <c r="F82" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="G82" s="8" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="83" spans="3:7">
+      <c r="C83" s="8" t="s">
+        <v>179</v>
+      </c>
+      <c r="D83" s="8" t="s">
+        <v>255</v>
+      </c>
+      <c r="E83" s="8"/>
+      <c r="F83" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="G83" s="8" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="84" spans="3:7">
+      <c r="C84" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="D84" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="E84" s="8">
+        <v>12</v>
+      </c>
+      <c r="F84" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="G84" s="8"/>
+    </row>
+    <row r="85" spans="3:7">
+      <c r="C85" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="D85" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="E85" s="8">
+        <v>50</v>
+      </c>
+      <c r="F85" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="G85" s="8"/>
+    </row>
+    <row r="86" spans="3:7">
+      <c r="C86" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="D86" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="E86" s="8"/>
+      <c r="F86" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="G86" s="8"/>
+    </row>
+    <row r="87" spans="3:7">
+      <c r="C87" s="8" t="s">
+        <v>257</v>
+      </c>
+      <c r="D87" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="E87" s="8"/>
+      <c r="F87" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="G87" s="8"/>
+    </row>
+    <row r="88" spans="3:7">
+      <c r="C88" s="8"/>
+      <c r="D88" s="8"/>
+      <c r="E88" s="8"/>
+      <c r="F88" s="8"/>
+      <c r="G88" s="8"/>
+    </row>
+    <row r="89" spans="3:7">
+      <c r="C89" s="8"/>
+      <c r="D89" s="8"/>
+      <c r="E89" s="8"/>
+      <c r="F89" s="8"/>
+      <c r="G89" s="8"/>
+    </row>
+    <row r="90" spans="3:7">
+      <c r="C90" s="7" t="s">
+        <v>245</v>
+      </c>
+      <c r="D90" s="7" t="s">
+        <v>258</v>
+      </c>
+      <c r="G90" s="11"/>
+    </row>
+    <row r="91" spans="3:7">
+      <c r="C91" s="9" t="s">
+        <v>247</v>
+      </c>
+      <c r="D91" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="E91" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="F91" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="G91" s="9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="92" spans="3:7">
+      <c r="C92" s="8" t="s">
+        <v>259</v>
+      </c>
+      <c r="D92" s="8" t="s">
+        <v>260</v>
+      </c>
+      <c r="E92" s="8"/>
+      <c r="F92" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="G92" s="8" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="93" spans="3:7">
+      <c r="C93" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="D93" s="8" t="s">
+        <v>260</v>
+      </c>
+      <c r="E93" s="8"/>
+      <c r="F93" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="G93" s="8" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="94" spans="3:7">
+      <c r="C94" s="8" t="s">
+        <v>263</v>
+      </c>
+      <c r="D94" s="8" t="s">
+        <v>264</v>
+      </c>
+      <c r="E94" s="8">
+        <v>30</v>
+      </c>
+      <c r="F94" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="G94" s="8" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="95" spans="3:7">
+      <c r="C95" s="8" t="s">
+        <v>266</v>
+      </c>
+      <c r="D95" s="8" t="s">
+        <v>267</v>
+      </c>
+      <c r="E95" s="8">
+        <v>50</v>
+      </c>
+      <c r="F95" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="G95" s="8"/>
+    </row>
+    <row r="96" spans="3:7">
+      <c r="C96" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="D96" s="8" t="s">
+        <v>268</v>
+      </c>
+      <c r="E96" s="8">
+        <v>12</v>
+      </c>
+      <c r="F96" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="G96" s="8"/>
+    </row>
+    <row r="97" spans="3:7">
+      <c r="C97" s="8" t="s">
+        <v>179</v>
+      </c>
+      <c r="D97" s="8" t="s">
+        <v>269</v>
+      </c>
+      <c r="E97" s="8"/>
+      <c r="F97" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="G97" s="8" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="98" spans="3:7">
+      <c r="C98" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="D98" s="8" t="s">
+        <v>271</v>
+      </c>
+      <c r="E98" s="8">
+        <v>200</v>
+      </c>
+      <c r="F98" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="G98" s="8"/>
+    </row>
+    <row r="99" spans="3:7">
+      <c r="C99" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="D99" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="E99" s="8"/>
+      <c r="F99" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="G99" s="8"/>
+    </row>
+    <row r="100" spans="3:7">
+      <c r="C100" s="8" t="s">
+        <v>257</v>
+      </c>
+      <c r="D100" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="E100" s="8"/>
+      <c r="F100" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="G100" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -5896,7 +6337,7 @@
   <sheetPr/>
   <dimension ref="B3:F56"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" workbookViewId="0">
+    <sheetView topLeftCell="A13" workbookViewId="0">
       <selection activeCell="B36" sqref="B36:F41"/>
     </sheetView>
   </sheetViews>
@@ -5909,189 +6350,189 @@
   <sheetData>
     <row r="3" spans="2:6">
       <c r="B3" t="s">
-        <v>245</v>
+        <v>272</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>84</v>
       </c>
       <c r="D3" t="s">
-        <v>246</v>
+        <v>273</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>84</v>
       </c>
       <c r="F3" t="s">
-        <v>247</v>
+        <v>274</v>
       </c>
     </row>
     <row r="4" spans="2:6">
       <c r="B4" t="s">
-        <v>245</v>
+        <v>272</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>85</v>
       </c>
       <c r="D4" t="s">
-        <v>246</v>
+        <v>273</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>85</v>
       </c>
       <c r="F4" t="s">
-        <v>247</v>
+        <v>274</v>
       </c>
     </row>
     <row r="5" spans="2:6">
       <c r="B5" t="s">
-        <v>245</v>
+        <v>272</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>87</v>
       </c>
       <c r="D5" t="s">
-        <v>246</v>
+        <v>273</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>87</v>
       </c>
       <c r="F5" t="s">
-        <v>247</v>
+        <v>274</v>
       </c>
     </row>
     <row r="6" spans="2:6">
       <c r="B6" t="s">
-        <v>245</v>
+        <v>272</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>88</v>
       </c>
       <c r="D6" t="s">
-        <v>246</v>
+        <v>273</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>88</v>
       </c>
       <c r="F6" t="s">
-        <v>247</v>
+        <v>274</v>
       </c>
     </row>
     <row r="7" spans="2:6">
       <c r="B7" t="s">
-        <v>245</v>
+        <v>272</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>89</v>
       </c>
       <c r="D7" t="s">
-        <v>246</v>
+        <v>273</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>89</v>
       </c>
       <c r="F7" t="s">
-        <v>247</v>
+        <v>274</v>
       </c>
     </row>
     <row r="8" spans="2:6">
       <c r="B8" t="s">
-        <v>245</v>
+        <v>272</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>91</v>
       </c>
       <c r="D8" t="s">
-        <v>246</v>
+        <v>273</v>
       </c>
       <c r="E8" s="1" t="s">
         <v>91</v>
       </c>
       <c r="F8" t="s">
-        <v>247</v>
+        <v>274</v>
       </c>
     </row>
     <row r="9" spans="2:6">
       <c r="B9" t="s">
-        <v>245</v>
+        <v>272</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>93</v>
       </c>
       <c r="D9" t="s">
-        <v>246</v>
+        <v>273</v>
       </c>
       <c r="E9" s="1" t="s">
         <v>93</v>
       </c>
       <c r="F9" t="s">
-        <v>247</v>
+        <v>274</v>
       </c>
     </row>
     <row r="10" spans="2:6">
       <c r="B10" t="s">
-        <v>245</v>
+        <v>272</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>94</v>
       </c>
       <c r="D10" t="s">
-        <v>246</v>
+        <v>273</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>94</v>
       </c>
       <c r="F10" t="s">
-        <v>247</v>
+        <v>274</v>
       </c>
     </row>
     <row r="11" spans="2:6">
       <c r="B11" t="s">
-        <v>245</v>
+        <v>272</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>95</v>
       </c>
       <c r="D11" t="s">
-        <v>246</v>
+        <v>273</v>
       </c>
       <c r="E11" s="1" t="s">
         <v>95</v>
       </c>
       <c r="F11" t="s">
-        <v>247</v>
+        <v>274</v>
       </c>
     </row>
     <row r="12" spans="2:6">
       <c r="B12" t="s">
-        <v>245</v>
+        <v>272</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>56</v>
       </c>
       <c r="D12" t="s">
-        <v>246</v>
+        <v>273</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>56</v>
       </c>
       <c r="F12" t="s">
-        <v>247</v>
+        <v>274</v>
       </c>
     </row>
     <row r="13" spans="2:6">
       <c r="B13" t="s">
-        <v>245</v>
+        <v>272</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>97</v>
       </c>
       <c r="D13" t="s">
-        <v>246</v>
+        <v>273</v>
       </c>
       <c r="E13" s="1" t="s">
         <v>97</v>
       </c>
       <c r="F13" t="s">
-        <v>247</v>
+        <v>274</v>
       </c>
     </row>
     <row r="14" spans="3:3">
@@ -6099,274 +6540,274 @@
     </row>
     <row r="16" spans="2:6">
       <c r="B16" t="s">
-        <v>245</v>
+        <v>272</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>99</v>
       </c>
       <c r="D16" t="s">
-        <v>248</v>
+        <v>275</v>
       </c>
       <c r="E16" s="1" t="s">
         <v>99</v>
       </c>
       <c r="F16" t="s">
-        <v>247</v>
+        <v>274</v>
       </c>
     </row>
     <row r="17" spans="2:6">
       <c r="B17" t="s">
-        <v>245</v>
+        <v>272</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>100</v>
       </c>
       <c r="D17" t="s">
-        <v>248</v>
+        <v>275</v>
       </c>
       <c r="E17" s="1" t="s">
         <v>100</v>
       </c>
       <c r="F17" t="s">
-        <v>247</v>
+        <v>274</v>
       </c>
     </row>
     <row r="18" spans="2:6">
       <c r="B18" t="s">
-        <v>245</v>
+        <v>272</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>101</v>
       </c>
       <c r="D18" t="s">
-        <v>248</v>
+        <v>275</v>
       </c>
       <c r="E18" s="1" t="s">
         <v>101</v>
       </c>
       <c r="F18" t="s">
-        <v>247</v>
+        <v>274</v>
       </c>
     </row>
     <row r="19" spans="2:6">
       <c r="B19" t="s">
-        <v>245</v>
+        <v>272</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>58</v>
       </c>
       <c r="D19" t="s">
-        <v>248</v>
+        <v>275</v>
       </c>
       <c r="E19" s="1" t="s">
         <v>58</v>
       </c>
       <c r="F19" t="s">
-        <v>247</v>
+        <v>274</v>
       </c>
     </row>
     <row r="20" spans="2:6">
       <c r="B20" t="s">
-        <v>245</v>
+        <v>272</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D20" t="s">
-        <v>248</v>
+        <v>275</v>
       </c>
       <c r="E20" s="1" t="s">
         <v>7</v>
       </c>
       <c r="F20" t="s">
-        <v>247</v>
+        <v>274</v>
       </c>
     </row>
     <row r="21" spans="2:6">
       <c r="B21" t="s">
-        <v>245</v>
+        <v>272</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>102</v>
       </c>
       <c r="D21" t="s">
-        <v>248</v>
+        <v>275</v>
       </c>
       <c r="E21" s="1" t="s">
         <v>102</v>
       </c>
       <c r="F21" t="s">
-        <v>247</v>
+        <v>274</v>
       </c>
     </row>
     <row r="22" spans="2:6">
       <c r="B22" t="s">
-        <v>245</v>
+        <v>272</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>103</v>
       </c>
       <c r="D22" t="s">
-        <v>248</v>
+        <v>275</v>
       </c>
       <c r="E22" s="1" t="s">
         <v>103</v>
       </c>
       <c r="F22" t="s">
-        <v>247</v>
+        <v>274</v>
       </c>
     </row>
     <row r="23" spans="2:6">
       <c r="B23" t="s">
-        <v>245</v>
+        <v>272</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>84</v>
       </c>
       <c r="D23" t="s">
-        <v>248</v>
+        <v>275</v>
       </c>
       <c r="E23" s="1" t="s">
         <v>84</v>
       </c>
       <c r="F23" t="s">
-        <v>247</v>
+        <v>274</v>
       </c>
     </row>
     <row r="26" spans="2:6">
       <c r="B26" t="s">
-        <v>245</v>
+        <v>272</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>208</v>
       </c>
       <c r="D26" t="s">
-        <v>249</v>
+        <v>276</v>
       </c>
       <c r="E26" s="1" t="s">
         <v>208</v>
       </c>
       <c r="F26" t="s">
-        <v>247</v>
+        <v>274</v>
       </c>
     </row>
     <row r="27" spans="2:6">
       <c r="B27" t="s">
-        <v>245</v>
+        <v>272</v>
       </c>
       <c r="C27" s="1" t="s">
         <v>209</v>
       </c>
       <c r="D27" t="s">
-        <v>249</v>
+        <v>276</v>
       </c>
       <c r="E27" s="1" t="s">
         <v>209</v>
       </c>
       <c r="F27" t="s">
-        <v>247</v>
+        <v>274</v>
       </c>
     </row>
     <row r="28" spans="2:6">
       <c r="B28" t="s">
-        <v>245</v>
+        <v>272</v>
       </c>
       <c r="C28" s="1" t="s">
         <v>212</v>
       </c>
       <c r="D28" t="s">
-        <v>249</v>
+        <v>276</v>
       </c>
       <c r="E28" s="1" t="s">
         <v>212</v>
       </c>
       <c r="F28" t="s">
-        <v>247</v>
+        <v>274</v>
       </c>
     </row>
     <row r="29" spans="2:6">
       <c r="B29" t="s">
-        <v>245</v>
+        <v>272</v>
       </c>
       <c r="C29" s="1" t="s">
         <v>215</v>
       </c>
       <c r="D29" t="s">
-        <v>249</v>
+        <v>276</v>
       </c>
       <c r="E29" s="1" t="s">
         <v>215</v>
       </c>
       <c r="F29" t="s">
-        <v>247</v>
+        <v>274</v>
       </c>
     </row>
     <row r="30" spans="2:6">
       <c r="B30" t="s">
-        <v>245</v>
+        <v>272</v>
       </c>
       <c r="C30" s="1" t="s">
         <v>217</v>
       </c>
       <c r="D30" t="s">
-        <v>249</v>
+        <v>276</v>
       </c>
       <c r="E30" s="1" t="s">
         <v>217</v>
       </c>
       <c r="F30" t="s">
-        <v>247</v>
+        <v>274</v>
       </c>
     </row>
     <row r="31" spans="2:6">
       <c r="B31" t="s">
-        <v>245</v>
+        <v>272</v>
       </c>
       <c r="C31" s="1" t="s">
         <v>219</v>
       </c>
       <c r="D31" t="s">
-        <v>249</v>
+        <v>276</v>
       </c>
       <c r="E31" s="1" t="s">
         <v>219</v>
       </c>
       <c r="F31" t="s">
-        <v>247</v>
+        <v>274</v>
       </c>
     </row>
     <row r="32" spans="2:6">
       <c r="B32" t="s">
-        <v>245</v>
+        <v>272</v>
       </c>
       <c r="C32" s="1" t="s">
         <v>221</v>
       </c>
       <c r="D32" t="s">
-        <v>249</v>
+        <v>276</v>
       </c>
       <c r="E32" s="1" t="s">
         <v>221</v>
       </c>
       <c r="F32" t="s">
-        <v>247</v>
+        <v>274</v>
       </c>
     </row>
     <row r="33" spans="2:6">
       <c r="B33" t="s">
-        <v>245</v>
+        <v>272</v>
       </c>
       <c r="C33" s="1" t="s">
         <v>179</v>
       </c>
       <c r="D33" t="s">
-        <v>249</v>
+        <v>276</v>
       </c>
       <c r="E33" s="1" t="s">
         <v>179</v>
       </c>
       <c r="F33" t="s">
-        <v>247</v>
+        <v>274</v>
       </c>
     </row>
     <row r="34" spans="3:3">
@@ -6374,236 +6815,236 @@
     </row>
     <row r="36" spans="2:6">
       <c r="B36" t="s">
-        <v>245</v>
+        <v>272</v>
       </c>
       <c r="C36" s="1" t="s">
         <v>224</v>
       </c>
       <c r="D36" t="s">
-        <v>250</v>
+        <v>277</v>
       </c>
       <c r="E36" s="1" t="s">
         <v>224</v>
       </c>
       <c r="F36" t="s">
-        <v>247</v>
+        <v>274</v>
       </c>
     </row>
     <row r="37" spans="2:6">
       <c r="B37" t="s">
-        <v>245</v>
+        <v>272</v>
       </c>
       <c r="C37" s="1" t="s">
         <v>208</v>
       </c>
       <c r="D37" t="s">
-        <v>250</v>
+        <v>277</v>
       </c>
       <c r="E37" s="1" t="s">
         <v>208</v>
       </c>
       <c r="F37" t="s">
-        <v>247</v>
+        <v>274</v>
       </c>
     </row>
     <row r="38" spans="2:6">
       <c r="B38" t="s">
-        <v>245</v>
+        <v>272</v>
       </c>
       <c r="C38" s="1" t="s">
         <v>84</v>
       </c>
       <c r="D38" t="s">
-        <v>250</v>
+        <v>277</v>
       </c>
       <c r="E38" s="1" t="s">
         <v>84</v>
       </c>
       <c r="F38" t="s">
-        <v>247</v>
+        <v>274</v>
       </c>
     </row>
     <row r="39" spans="2:6">
       <c r="B39" t="s">
-        <v>245</v>
+        <v>272</v>
       </c>
       <c r="C39" s="4" t="s">
         <v>227</v>
       </c>
       <c r="D39" t="s">
-        <v>250</v>
+        <v>277</v>
       </c>
       <c r="E39" s="4" t="s">
         <v>227</v>
       </c>
       <c r="F39" t="s">
-        <v>247</v>
+        <v>274</v>
       </c>
     </row>
     <row r="40" spans="2:6">
       <c r="B40" t="s">
-        <v>245</v>
+        <v>272</v>
       </c>
       <c r="C40" s="4" t="s">
         <v>229</v>
       </c>
       <c r="D40" t="s">
-        <v>250</v>
+        <v>277</v>
       </c>
       <c r="E40" s="4" t="s">
         <v>229</v>
       </c>
       <c r="F40" t="s">
-        <v>247</v>
+        <v>274</v>
       </c>
     </row>
     <row r="41" spans="2:6">
       <c r="B41" t="s">
-        <v>245</v>
+        <v>272</v>
       </c>
       <c r="C41" s="4" t="s">
         <v>179</v>
       </c>
       <c r="D41" t="s">
-        <v>250</v>
+        <v>277</v>
       </c>
       <c r="E41" s="4" t="s">
         <v>179</v>
       </c>
       <c r="F41" t="s">
-        <v>247</v>
+        <v>274</v>
       </c>
     </row>
     <row r="45" spans="2:4">
       <c r="B45" t="s">
-        <v>245</v>
+        <v>272</v>
       </c>
       <c r="C45" s="1" t="s">
         <v>234</v>
       </c>
       <c r="D45" t="s">
-        <v>251</v>
+        <v>278</v>
       </c>
     </row>
     <row r="46" spans="2:4">
       <c r="B46" t="s">
-        <v>245</v>
+        <v>272</v>
       </c>
       <c r="C46" s="1" t="s">
         <v>209</v>
       </c>
       <c r="D46" t="s">
-        <v>251</v>
+        <v>278</v>
       </c>
     </row>
     <row r="47" spans="2:4">
       <c r="B47" t="s">
-        <v>245</v>
+        <v>272</v>
       </c>
       <c r="C47" s="4" t="s">
         <v>235</v>
       </c>
       <c r="D47" t="s">
-        <v>251</v>
+        <v>278</v>
       </c>
     </row>
     <row r="48" spans="2:4">
       <c r="B48" t="s">
-        <v>245</v>
+        <v>272</v>
       </c>
       <c r="C48" s="4" t="s">
         <v>237</v>
       </c>
       <c r="D48" t="s">
-        <v>251</v>
+        <v>278</v>
       </c>
     </row>
     <row r="49" spans="2:4">
       <c r="B49" t="s">
-        <v>245</v>
+        <v>272</v>
       </c>
       <c r="C49" s="4" t="s">
         <v>238</v>
       </c>
       <c r="D49" t="s">
-        <v>251</v>
+        <v>278</v>
       </c>
     </row>
     <row r="50" spans="2:4">
       <c r="B50" t="s">
-        <v>245</v>
+        <v>272</v>
       </c>
       <c r="C50" s="4" t="s">
         <v>239</v>
       </c>
       <c r="D50" t="s">
-        <v>251</v>
+        <v>278</v>
       </c>
     </row>
     <row r="51" spans="2:4">
       <c r="B51" t="s">
-        <v>245</v>
+        <v>272</v>
       </c>
       <c r="C51" s="4" t="s">
         <v>240</v>
       </c>
       <c r="D51" t="s">
-        <v>251</v>
+        <v>278</v>
       </c>
     </row>
     <row r="52" spans="2:4">
       <c r="B52" t="s">
-        <v>245</v>
+        <v>272</v>
       </c>
       <c r="C52" s="4" t="s">
         <v>241</v>
       </c>
       <c r="D52" t="s">
-        <v>251</v>
+        <v>278</v>
       </c>
     </row>
     <row r="53" spans="2:4">
       <c r="B53" t="s">
-        <v>245</v>
+        <v>272</v>
       </c>
       <c r="C53" s="4" t="s">
         <v>242</v>
       </c>
       <c r="D53" t="s">
-        <v>251</v>
+        <v>278</v>
       </c>
     </row>
     <row r="54" spans="2:4">
       <c r="B54" t="s">
-        <v>245</v>
+        <v>272</v>
       </c>
       <c r="C54" s="4" t="s">
         <v>243</v>
       </c>
       <c r="D54" t="s">
-        <v>251</v>
+        <v>278</v>
       </c>
     </row>
     <row r="55" spans="2:4">
       <c r="B55" t="s">
-        <v>245</v>
+        <v>272</v>
       </c>
       <c r="C55" s="4" t="s">
         <v>244</v>
       </c>
       <c r="D55" t="s">
-        <v>251</v>
+        <v>278</v>
       </c>
     </row>
     <row r="56" spans="2:4">
       <c r="B56" t="s">
-        <v>245</v>
+        <v>272</v>
       </c>
       <c r="C56" s="4" t="s">
         <v>53</v>
       </c>
       <c r="D56" t="s">
-        <v>251</v>
+        <v>278</v>
       </c>
     </row>
   </sheetData>

</xml_diff>